<commit_message>
REF/SM: Update snapshot templates.
</commit_message>
<xml_diff>
--- a/phantasy_apps/settings_manager/contrib/templates/template_LINAC_ARIS.xlsx
+++ b/phantasy_apps/settings_manager/contrib/templates/template_LINAC_ARIS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7718" uniqueCount="999">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7703" uniqueCount="1008">
   <si>
     <t xml:space="preserve">timestamp</t>
   </si>
@@ -2909,12 +2909,21 @@
     <t xml:space="preserve">FS_F1S1:Q_D1024</t>
   </si>
   <si>
+    <t xml:space="preserve">FS_F1S1:OCT_D1024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OCT</t>
+  </si>
+  <si>
     <t xml:space="preserve">FS_F1S1:S_D1024</t>
   </si>
   <si>
     <t xml:space="preserve">FS_F1S1:Q_D1035</t>
   </si>
   <si>
+    <t xml:space="preserve">FS_F1S1:OCT_D1035</t>
+  </si>
+  <si>
     <t xml:space="preserve">FS_F1S1:S_D1035</t>
   </si>
   <si>
@@ -2927,36 +2936,54 @@
     <t xml:space="preserve">FS_F1S1:Q_D1137</t>
   </si>
   <si>
+    <t xml:space="preserve">FS_F1S1:OCT_D1137</t>
+  </si>
+  <si>
     <t xml:space="preserve">FS_F1S1:S_D1137</t>
   </si>
   <si>
     <t xml:space="preserve">FS_F1S1:Q_D1148</t>
   </si>
   <si>
+    <t xml:space="preserve">FS_F1S1:OCT_D1148</t>
+  </si>
+  <si>
     <t xml:space="preserve">FS_F1S1:S_D1148</t>
   </si>
   <si>
     <t xml:space="preserve">FS_F1S1:Q_D1170</t>
   </si>
   <si>
+    <t xml:space="preserve">FS_F1S1:OCT_D1170</t>
+  </si>
+  <si>
     <t xml:space="preserve">FS_F1S1:S_D1170</t>
   </si>
   <si>
     <t xml:space="preserve">FS_F1S2:Q_D1195</t>
   </si>
   <si>
+    <t xml:space="preserve">FS_F1S2:OCT_D1195</t>
+  </si>
+  <si>
     <t xml:space="preserve">FS_F1S2:S_D1195</t>
   </si>
   <si>
     <t xml:space="preserve">FS_F1S2:Q_D1207</t>
   </si>
   <si>
+    <t xml:space="preserve">FS_F1S2:OCT_D1207</t>
+  </si>
+  <si>
     <t xml:space="preserve">FS_F1S2:S_D1207</t>
   </si>
   <si>
     <t xml:space="preserve">FS_F1S2:Q_D1218</t>
   </si>
   <si>
+    <t xml:space="preserve">FS_F1S2:OCT_D1218</t>
+  </si>
+  <si>
     <t xml:space="preserve">FS_F1S2:S_D1218</t>
   </si>
   <si>
@@ -2966,58 +2993,58 @@
     <t xml:space="preserve">FS_F1S2:Q_D1288</t>
   </si>
   <si>
+    <t xml:space="preserve">FS_F1S2:OCT_D1288</t>
+  </si>
+  <si>
     <t xml:space="preserve">FS_F1S2:S_D1288</t>
   </si>
   <si>
     <t xml:space="preserve">FS_F1S2:Q_D1299</t>
   </si>
   <si>
+    <t xml:space="preserve">FS_F1S2:OCT_D1299</t>
+  </si>
+  <si>
     <t xml:space="preserve">FS_F1S2:S_D1299</t>
   </si>
   <si>
     <t xml:space="preserve">FS_F1S2:Q_D1311</t>
   </si>
   <si>
+    <t xml:space="preserve">FS_F1S2:OCT_D1311</t>
+  </si>
+  <si>
     <t xml:space="preserve">FS_F1S2:S_D1311</t>
   </si>
   <si>
     <t xml:space="preserve">FS_F1S2:Q_D1338</t>
   </si>
   <si>
+    <t xml:space="preserve">FS_F1S2:OCT_D1338</t>
+  </si>
+  <si>
     <t xml:space="preserve">FS_F1S2:S_D1338</t>
   </si>
   <si>
     <t xml:space="preserve">FS_F1S2:Q_D1349</t>
   </si>
   <si>
+    <t xml:space="preserve">FS_F1S2:OCT_D1349</t>
+  </si>
+  <si>
     <t xml:space="preserve">FS_F1S2:S_D1349</t>
   </si>
   <si>
     <t xml:space="preserve">FS_F1S2:Q_D1361</t>
   </si>
   <si>
+    <t xml:space="preserve">FS_F1S2:OCT_D1361</t>
+  </si>
+  <si>
     <t xml:space="preserve">FS_F1S2:S_D1361</t>
   </si>
   <si>
     <t xml:space="preserve">FS_F1S2:DV_D1402</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FS_F1S2:Q_D1430</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FS_F1S2:S_D1430</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FS_F1S2:Q_D1441</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FS_F1S2:S_D1441</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FS_F1S2:Q_D1453</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FS_F1S2:S_D1453</t>
   </si>
 </sst>
 </file>
@@ -3129,19 +3156,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3266,8 +3295,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3276,19 +3305,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1856" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1883" activeCellId="0" sqref="A1883"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1875" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1891" activeCellId="0" sqref="D1891"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="8.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40956,12 +40986,6 @@
       <c r="D1883" s="0" t="n">
         <v>0.9882</v>
       </c>
-      <c r="H1883" s="0" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="I1883" s="0" t="s">
-        <v>47</v>
-      </c>
     </row>
     <row r="1884" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1884" s="0" t="s">
@@ -40976,12 +41000,6 @@
       <c r="D1884" s="0" t="n">
         <v>1.976</v>
       </c>
-      <c r="H1884" s="0" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="I1884" s="0" t="s">
-        <v>47</v>
-      </c>
     </row>
     <row r="1885" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1885" s="0" t="s">
@@ -40991,141 +41009,99 @@
         <v>55</v>
       </c>
       <c r="C1885" s="0" t="s">
-        <v>472</v>
+        <v>963</v>
       </c>
       <c r="D1885" s="0" t="n">
         <v>2.375</v>
       </c>
-      <c r="H1885" s="0" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="I1885" s="0" t="s">
-        <v>47</v>
-      </c>
     </row>
     <row r="1886" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1886" s="0" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="B1886" s="0" t="s">
         <v>55</v>
       </c>
       <c r="C1886" s="0" t="s">
-        <v>161</v>
+        <v>472</v>
       </c>
       <c r="D1886" s="0" t="n">
-        <v>3.076</v>
-      </c>
-      <c r="H1886" s="0" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="I1886" s="0" t="s">
-        <v>47</v>
+        <v>2.375</v>
       </c>
     </row>
     <row r="1887" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1887" s="0" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="B1887" s="0" t="s">
         <v>55</v>
       </c>
       <c r="C1887" s="0" t="s">
-        <v>472</v>
+        <v>161</v>
       </c>
       <c r="D1887" s="0" t="n">
-        <v>3.475</v>
-      </c>
-      <c r="H1887" s="0" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="I1887" s="0" t="s">
-        <v>47</v>
+        <v>3.076</v>
       </c>
     </row>
     <row r="1888" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1888" s="0" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="B1888" s="0" t="s">
         <v>55</v>
       </c>
       <c r="C1888" s="0" t="s">
-        <v>74</v>
+        <v>963</v>
       </c>
       <c r="D1888" s="0" t="n">
-        <v>5.4</v>
-      </c>
-      <c r="H1888" s="0" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="I1888" s="0" t="s">
-        <v>47</v>
+        <v>3.475</v>
       </c>
     </row>
     <row r="1889" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1889" s="0" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c r="B1889" s="0" t="s">
         <v>55</v>
       </c>
       <c r="C1889" s="0" t="s">
-        <v>74</v>
+        <v>472</v>
       </c>
       <c r="D1889" s="0" t="n">
-        <v>9.7704</v>
-      </c>
-      <c r="H1889" s="0" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="I1889" s="0" t="s">
-        <v>47</v>
+        <v>3.475</v>
       </c>
     </row>
     <row r="1890" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1890" s="0" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="B1890" s="0" t="s">
         <v>55</v>
       </c>
       <c r="C1890" s="0" t="s">
-        <v>161</v>
+        <v>74</v>
       </c>
       <c r="D1890" s="0" t="n">
-        <v>13.2533</v>
-      </c>
-      <c r="H1890" s="0" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="I1890" s="0" t="s">
-        <v>47</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="1891" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1891" s="0" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="B1891" s="0" t="s">
         <v>55</v>
       </c>
       <c r="C1891" s="0" t="s">
-        <v>472</v>
+        <v>74</v>
       </c>
       <c r="D1891" s="0" t="n">
-        <v>13.6638</v>
-      </c>
-      <c r="H1891" s="0" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="I1891" s="0" t="s">
-        <v>47</v>
+        <v>9.7704</v>
       </c>
     </row>
     <row r="1892" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1892" s="0" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="B1892" s="0" t="s">
         <v>55</v>
@@ -41134,98 +41110,68 @@
         <v>161</v>
       </c>
       <c r="D1892" s="0" t="n">
-        <v>14.341</v>
-      </c>
-      <c r="H1892" s="0" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="I1892" s="0" t="s">
-        <v>47</v>
+        <v>13.2533</v>
       </c>
     </row>
     <row r="1893" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1893" s="0" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="B1893" s="0" t="s">
         <v>55</v>
       </c>
       <c r="C1893" s="0" t="s">
-        <v>472</v>
+        <v>963</v>
       </c>
       <c r="D1893" s="0" t="n">
-        <v>14.7515</v>
-      </c>
-      <c r="H1893" s="0" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="I1893" s="0" t="s">
-        <v>47</v>
+        <v>13.6638</v>
       </c>
     </row>
     <row r="1894" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1894" s="0" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="B1894" s="0" t="s">
         <v>55</v>
       </c>
       <c r="C1894" s="0" t="s">
-        <v>161</v>
+        <v>472</v>
       </c>
       <c r="D1894" s="0" t="n">
-        <v>16.6283</v>
-      </c>
-      <c r="H1894" s="0" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="I1894" s="0" t="s">
-        <v>47</v>
+        <v>13.6638</v>
       </c>
     </row>
     <row r="1895" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1895" s="0" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="B1895" s="0" t="s">
         <v>55</v>
       </c>
       <c r="C1895" s="0" t="s">
-        <v>472</v>
+        <v>161</v>
       </c>
       <c r="D1895" s="0" t="n">
-        <v>17.0388</v>
-      </c>
-      <c r="H1895" s="0" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="I1895" s="0" t="s">
-        <v>47</v>
+        <v>14.341</v>
       </c>
     </row>
     <row r="1896" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1896" s="0" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B1896" s="0" t="s">
         <v>55</v>
       </c>
       <c r="C1896" s="0" t="s">
-        <v>161</v>
+        <v>963</v>
       </c>
       <c r="D1896" s="0" t="n">
-        <v>19.1764</v>
-      </c>
-      <c r="H1896" s="0" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="I1896" s="0" t="s">
-        <v>47</v>
+        <v>14.7515</v>
       </c>
     </row>
     <row r="1897" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1897" s="0" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="B1897" s="0" t="s">
         <v>55</v>
@@ -41234,18 +41180,12 @@
         <v>472</v>
       </c>
       <c r="D1897" s="0" t="n">
-        <v>19.5293</v>
-      </c>
-      <c r="H1897" s="0" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="I1897" s="0" t="s">
-        <v>47</v>
+        <v>14.7515</v>
       </c>
     </row>
     <row r="1898" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1898" s="0" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="B1898" s="0" t="s">
         <v>55</v>
@@ -41254,158 +41194,110 @@
         <v>161</v>
       </c>
       <c r="D1898" s="0" t="n">
-        <v>20.2146</v>
-      </c>
-      <c r="H1898" s="0" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="I1898" s="0" t="s">
-        <v>47</v>
+        <v>16.6283</v>
       </c>
     </row>
     <row r="1899" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1899" s="0" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="B1899" s="0" t="s">
         <v>55</v>
       </c>
       <c r="C1899" s="0" t="s">
-        <v>472</v>
+        <v>963</v>
       </c>
       <c r="D1899" s="0" t="n">
-        <v>20.6515</v>
-      </c>
-      <c r="H1899" s="0" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="I1899" s="0" t="s">
-        <v>47</v>
+        <v>17.0388</v>
       </c>
     </row>
     <row r="1900" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1900" s="0" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
       <c r="B1900" s="0" t="s">
         <v>55</v>
       </c>
       <c r="C1900" s="0" t="s">
-        <v>161</v>
+        <v>472</v>
       </c>
       <c r="D1900" s="0" t="n">
-        <v>21.4208</v>
-      </c>
-      <c r="H1900" s="0" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="I1900" s="0" t="s">
-        <v>47</v>
+        <v>17.0388</v>
       </c>
     </row>
     <row r="1901" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1901" s="0" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="B1901" s="0" t="s">
         <v>55</v>
       </c>
       <c r="C1901" s="0" t="s">
-        <v>472</v>
+        <v>161</v>
       </c>
       <c r="D1901" s="0" t="n">
-        <v>21.7737</v>
-      </c>
-      <c r="H1901" s="0" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="I1901" s="0" t="s">
-        <v>47</v>
+        <v>19.1764</v>
       </c>
     </row>
     <row r="1902" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1902" s="0" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="B1902" s="0" t="s">
         <v>55</v>
       </c>
       <c r="C1902" s="0" t="s">
-        <v>74</v>
+        <v>963</v>
       </c>
       <c r="D1902" s="0" t="n">
-        <v>22.8963</v>
-      </c>
-      <c r="H1902" s="0" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="I1902" s="0" t="s">
-        <v>47</v>
+        <v>19.5293</v>
       </c>
     </row>
     <row r="1903" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1903" s="0" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="B1903" s="0" t="s">
         <v>55</v>
       </c>
       <c r="C1903" s="0" t="s">
-        <v>161</v>
+        <v>472</v>
       </c>
       <c r="D1903" s="0" t="n">
-        <v>28.4512</v>
-      </c>
-      <c r="H1903" s="0" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="I1903" s="0" t="s">
-        <v>47</v>
+        <v>19.5293</v>
       </c>
     </row>
     <row r="1904" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1904" s="0" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="B1904" s="0" t="s">
         <v>55</v>
       </c>
       <c r="C1904" s="0" t="s">
-        <v>472</v>
+        <v>161</v>
       </c>
       <c r="D1904" s="0" t="n">
-        <v>28.804</v>
-      </c>
-      <c r="H1904" s="0" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="I1904" s="0" t="s">
-        <v>47</v>
+        <v>20.2146</v>
       </c>
     </row>
     <row r="1905" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1905" s="0" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="B1905" s="0" t="s">
         <v>55</v>
       </c>
       <c r="C1905" s="0" t="s">
-        <v>161</v>
+        <v>963</v>
       </c>
       <c r="D1905" s="0" t="n">
-        <v>29.4894</v>
-      </c>
-      <c r="H1905" s="0" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="I1905" s="0" t="s">
-        <v>47</v>
+        <v>20.6515</v>
       </c>
     </row>
     <row r="1906" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1906" s="0" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B1906" s="0" t="s">
         <v>55</v>
@@ -41414,18 +41306,12 @@
         <v>472</v>
       </c>
       <c r="D1906" s="0" t="n">
-        <v>29.9263</v>
-      </c>
-      <c r="H1906" s="0" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="I1906" s="0" t="s">
-        <v>47</v>
+        <v>20.6515</v>
       </c>
     </row>
     <row r="1907" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1907" s="0" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="B1907" s="0" t="s">
         <v>55</v>
@@ -41434,78 +41320,54 @@
         <v>161</v>
       </c>
       <c r="D1907" s="0" t="n">
-        <v>30.6956</v>
-      </c>
-      <c r="H1907" s="0" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="I1907" s="0" t="s">
-        <v>47</v>
+        <v>21.4208</v>
       </c>
     </row>
     <row r="1908" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1908" s="0" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="B1908" s="0" t="s">
         <v>55</v>
       </c>
       <c r="C1908" s="0" t="s">
-        <v>472</v>
+        <v>963</v>
       </c>
       <c r="D1908" s="0" t="n">
-        <v>31.0485</v>
-      </c>
-      <c r="H1908" s="0" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="I1908" s="0" t="s">
-        <v>47</v>
+        <v>21.7737</v>
       </c>
     </row>
     <row r="1909" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1909" s="0" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="B1909" s="0" t="s">
         <v>55</v>
       </c>
       <c r="C1909" s="0" t="s">
-        <v>161</v>
+        <v>472</v>
       </c>
       <c r="D1909" s="0" t="n">
-        <v>33.4581</v>
-      </c>
-      <c r="H1909" s="0" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="I1909" s="0" t="s">
-        <v>47</v>
+        <v>21.7737</v>
       </c>
     </row>
     <row r="1910" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1910" s="0" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="B1910" s="0" t="s">
         <v>55</v>
       </c>
       <c r="C1910" s="0" t="s">
-        <v>472</v>
+        <v>74</v>
       </c>
       <c r="D1910" s="0" t="n">
-        <v>33.811</v>
-      </c>
-      <c r="H1910" s="0" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="I1910" s="0" t="s">
-        <v>47</v>
+        <v>22.8963</v>
       </c>
     </row>
     <row r="1911" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1911" s="0" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="B1911" s="0" t="s">
         <v>55</v>
@@ -41514,158 +41376,110 @@
         <v>161</v>
       </c>
       <c r="D1911" s="0" t="n">
-        <v>34.4963</v>
-      </c>
-      <c r="H1911" s="0" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="I1911" s="0" t="s">
-        <v>47</v>
+        <v>28.4512</v>
       </c>
     </row>
     <row r="1912" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1912" s="0" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="B1912" s="0" t="s">
         <v>55</v>
       </c>
       <c r="C1912" s="0" t="s">
-        <v>472</v>
+        <v>963</v>
       </c>
       <c r="D1912" s="0" t="n">
-        <v>34.9332</v>
-      </c>
-      <c r="H1912" s="0" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="I1912" s="0" t="s">
-        <v>47</v>
+        <v>28.804</v>
       </c>
     </row>
     <row r="1913" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1913" s="0" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="B1913" s="0" t="s">
         <v>55</v>
       </c>
       <c r="C1913" s="0" t="s">
-        <v>161</v>
+        <v>472</v>
       </c>
       <c r="D1913" s="0" t="n">
-        <v>35.7025</v>
-      </c>
-      <c r="H1913" s="0" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="I1913" s="0" t="s">
-        <v>47</v>
+        <v>28.804</v>
       </c>
     </row>
     <row r="1914" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1914" s="0" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="B1914" s="0" t="s">
         <v>55</v>
       </c>
       <c r="C1914" s="0" t="s">
-        <v>472</v>
+        <v>161</v>
       </c>
       <c r="D1914" s="0" t="n">
-        <v>36.0554</v>
-      </c>
-      <c r="H1914" s="0" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="I1914" s="0" t="s">
-        <v>47</v>
+        <v>29.4894</v>
       </c>
     </row>
     <row r="1915" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1915" s="0" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="B1915" s="0" t="s">
         <v>55</v>
       </c>
       <c r="C1915" s="0" t="s">
-        <v>74</v>
+        <v>963</v>
       </c>
       <c r="D1915" s="0" t="n">
-        <v>38.4725</v>
-      </c>
-      <c r="H1915" s="0" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="I1915" s="0" t="s">
-        <v>47</v>
+        <v>29.9263</v>
       </c>
     </row>
     <row r="1916" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1916" s="0" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B1916" s="0" t="s">
         <v>55</v>
       </c>
       <c r="C1916" s="0" t="s">
-        <v>161</v>
+        <v>472</v>
       </c>
       <c r="D1916" s="0" t="n">
-        <v>42.7063</v>
-      </c>
-      <c r="H1916" s="0" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="I1916" s="0" t="s">
-        <v>47</v>
+        <v>29.9263</v>
       </c>
     </row>
     <row r="1917" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1917" s="0" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="B1917" s="0" t="s">
         <v>55</v>
       </c>
       <c r="C1917" s="0" t="s">
-        <v>472</v>
+        <v>161</v>
       </c>
       <c r="D1917" s="0" t="n">
-        <v>43.021</v>
-      </c>
-      <c r="H1917" s="0" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="I1917" s="0" t="s">
-        <v>47</v>
+        <v>30.6956</v>
       </c>
     </row>
     <row r="1918" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1918" s="0" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="B1918" s="0" t="s">
         <v>55</v>
       </c>
       <c r="C1918" s="0" t="s">
-        <v>161</v>
+        <v>963</v>
       </c>
       <c r="D1918" s="0" t="n">
-        <v>43.7297</v>
-      </c>
-      <c r="H1918" s="0" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="I1918" s="0" t="s">
-        <v>47</v>
+        <v>31.0485</v>
       </c>
     </row>
     <row r="1919" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1919" s="0" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="B1919" s="0" t="s">
         <v>55</v>
@@ -41674,18 +41488,12 @@
         <v>472</v>
       </c>
       <c r="D1919" s="0" t="n">
-        <v>44.1397</v>
-      </c>
-      <c r="H1919" s="0" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="I1919" s="0" t="s">
-        <v>47</v>
+        <v>31.0485</v>
       </c>
     </row>
     <row r="1920" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1920" s="0" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="B1920" s="0" t="s">
         <v>55</v>
@@ -41694,40 +41502,140 @@
         <v>161</v>
       </c>
       <c r="D1920" s="0" t="n">
-        <v>44.9437</v>
-      </c>
-      <c r="H1920" s="0" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="I1920" s="0" t="s">
-        <v>47</v>
+        <v>33.4581</v>
       </c>
     </row>
     <row r="1921" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1921" s="0" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="B1921" s="0" t="s">
         <v>55</v>
       </c>
       <c r="C1921" s="0" t="s">
+        <v>963</v>
+      </c>
+      <c r="D1921" s="0" t="n">
+        <v>33.811</v>
+      </c>
+    </row>
+    <row r="1922" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1922" s="0" t="s">
+        <v>1000</v>
+      </c>
+      <c r="B1922" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1922" s="0" t="s">
         <v>472</v>
       </c>
-      <c r="D1921" s="0" t="n">
-        <v>45.2584</v>
-      </c>
-      <c r="H1921" s="0" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="I1921" s="0" t="s">
-        <v>47</v>
+      <c r="D1922" s="0" t="n">
+        <v>33.811</v>
+      </c>
+    </row>
+    <row r="1923" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1923" s="0" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B1923" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1923" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="D1923" s="0" t="n">
+        <v>34.4963</v>
+      </c>
+    </row>
+    <row r="1924" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1924" s="0" t="s">
+        <v>1002</v>
+      </c>
+      <c r="B1924" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1924" s="0" t="s">
+        <v>963</v>
+      </c>
+      <c r="D1924" s="0" t="n">
+        <v>34.9332</v>
+      </c>
+    </row>
+    <row r="1925" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1925" s="0" t="s">
+        <v>1003</v>
+      </c>
+      <c r="B1925" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1925" s="0" t="s">
+        <v>472</v>
+      </c>
+      <c r="D1925" s="0" t="n">
+        <v>34.9332</v>
+      </c>
+    </row>
+    <row r="1926" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1926" s="0" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B1926" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1926" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="D1926" s="0" t="n">
+        <v>35.7025</v>
+      </c>
+    </row>
+    <row r="1927" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1927" s="0" t="s">
+        <v>1005</v>
+      </c>
+      <c r="B1927" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1927" s="0" t="s">
+        <v>963</v>
+      </c>
+      <c r="D1927" s="0" t="n">
+        <v>36.0554</v>
+      </c>
+    </row>
+    <row r="1928" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1928" s="0" t="s">
+        <v>1006</v>
+      </c>
+      <c r="B1928" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1928" s="0" t="s">
+        <v>472</v>
+      </c>
+      <c r="D1928" s="0" t="n">
+        <v>36.0554</v>
+      </c>
+    </row>
+    <row r="1929" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1929" s="0" t="s">
+        <v>1007</v>
+      </c>
+      <c r="B1929" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1929" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1929" s="0" t="n">
+        <v>38.4725</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>